<commit_message>
trying to get weights for 1d
</commit_message>
<xml_diff>
--- a/APPENDIX DATA.xlsx
+++ b/APPENDIX DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/UNI/Y3/HSBC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D3041B-9648-E547-BCE9-93528591D9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD26F6E-A5C8-BB43-9FF7-AA7E11EF61EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="155">
   <si>
     <t>Appendix D: High Conviction Fund List</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t>Fund</t>
+  </si>
+  <si>
+    <t>Sharpe Ratio</t>
   </si>
 </sst>
 </file>
@@ -6228,15 +6231,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C2DA5B-98AD-F549-ABC3-D1EC9E9B0836}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="33" t="s">
         <v>148</v>
       </c>
@@ -6258,8 +6261,11 @@
       <c r="G1" s="33" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="24" t="s">
         <v>11</v>
       </c>
@@ -6281,8 +6287,11 @@
       <c r="G2" s="24">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="24">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="24" t="s">
         <v>11</v>
       </c>
@@ -6304,8 +6313,11 @@
       <c r="G3" s="24">
         <v>11.19</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="24" t="s">
         <v>11</v>
       </c>
@@ -6325,10 +6337,13 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="G4" s="24">
-        <v>10.65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>9.64</v>
+      </c>
+      <c r="H4" s="24">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="24" t="s">
         <v>11</v>
       </c>
@@ -6348,10 +6363,13 @@
         <v>0.61</v>
       </c>
       <c r="G5" s="24">
-        <v>7.62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>7.8</v>
+      </c>
+      <c r="H5" s="24">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="24" t="s">
         <v>11</v>
       </c>
@@ -6371,10 +6389,13 @@
         <v>0.99</v>
       </c>
       <c r="G6" s="24">
-        <v>9.8800000000000008</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>11.72</v>
+      </c>
+      <c r="H6" s="24">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="24" t="s">
         <v>11</v>
       </c>
@@ -6394,10 +6415,13 @@
         <v>0.77</v>
       </c>
       <c r="G7" s="24">
-        <v>8.57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="H7" s="24">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="24" t="s">
         <v>11</v>
       </c>
@@ -6417,10 +6441,13 @@
         <v>0.8</v>
       </c>
       <c r="G8" s="24">
-        <v>8.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="24" t="s">
         <v>11</v>
       </c>
@@ -6442,8 +6469,11 @@
       <c r="G9" s="24">
         <v>9.82</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="24">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="24" t="s">
         <v>11</v>
       </c>
@@ -6463,10 +6493,13 @@
         <v>0.71</v>
       </c>
       <c r="G10" s="24">
-        <v>8.2200000000000006</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>8.93</v>
+      </c>
+      <c r="H10" s="24">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="24" t="s">
         <v>11</v>
       </c>
@@ -6488,8 +6521,11 @@
       <c r="G11" s="24">
         <v>8.6300000000000008</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="24">
+        <v>-0.31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="24" t="s">
         <v>11</v>
       </c>
@@ -6509,10 +6545,13 @@
         <v>0.89</v>
       </c>
       <c r="G12" s="24">
-        <v>9.2899999999999991</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>9.82</v>
+      </c>
+      <c r="H12" s="24">
+        <v>-0.19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="24" t="s">
         <v>11</v>
       </c>
@@ -6532,10 +6571,13 @@
         <v>0.93</v>
       </c>
       <c r="G13" s="24">
-        <v>9.52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="H13" s="24">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="24" t="s">
         <v>11</v>
       </c>
@@ -6555,10 +6597,13 @@
         <v>0.85</v>
       </c>
       <c r="G14" s="24">
-        <v>9.0500000000000007</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>8.99</v>
+      </c>
+      <c r="H14" s="24">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="24" t="s">
         <v>11</v>
       </c>
@@ -6578,10 +6623,13 @@
         <v>1.08</v>
       </c>
       <c r="G15" s="24">
-        <v>10.42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>10.71</v>
+      </c>
+      <c r="H15" s="24">
+        <v>-0.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="24" t="s">
         <v>11</v>
       </c>
@@ -6603,8 +6651,11 @@
       <c r="G16" s="24">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="24">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="24" t="s">
         <v>11</v>
       </c>
@@ -6624,10 +6675,13 @@
         <v>0.87</v>
       </c>
       <c r="G17" s="24">
-        <v>9.17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="24" t="s">
         <v>11</v>
       </c>
@@ -6649,8 +6703,11 @@
       <c r="G18" s="24">
         <v>9.2899999999999991</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" s="24">
+        <v>-1.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="24" t="s">
         <v>11</v>
       </c>
@@ -6670,10 +6727,13 @@
         <v>1.19</v>
       </c>
       <c r="G19" s="24">
-        <v>11.07</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>9.17</v>
+      </c>
+      <c r="H19" s="24">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="24" t="s">
         <v>11</v>
       </c>
@@ -6695,8 +6755,11 @@
       <c r="G20" s="24">
         <v>4.16</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="24">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="24" t="s">
         <v>11</v>
       </c>
@@ -6718,8 +6781,11 @@
       <c r="G21" s="24">
         <v>10.06</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" s="24">
+        <v>-0.61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="24" t="s">
         <v>11</v>
       </c>
@@ -6739,10 +6805,13 @@
         <v>0.79</v>
       </c>
       <c r="G22" s="24">
-        <v>8.69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>8.51</v>
+      </c>
+      <c r="H22" s="24">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="24" t="s">
         <v>11</v>
       </c>
@@ -6764,8 +6833,11 @@
       <c r="G23" s="24">
         <v>5.32</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="24">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="24" t="s">
         <v>11</v>
       </c>
@@ -6787,8 +6859,11 @@
       <c r="G24" s="24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="24">
+        <v>-1.59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="24" t="s">
         <v>71</v>
       </c>
@@ -6808,10 +6883,13 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="G25" s="24">
-        <v>10.77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>10.53</v>
+      </c>
+      <c r="H25" s="24">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="24" t="s">
         <v>71</v>
       </c>
@@ -6831,10 +6909,13 @@
         <v>0.79</v>
       </c>
       <c r="G26" s="24">
-        <v>8.69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>9.64</v>
+      </c>
+      <c r="H26" s="24">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="24" t="s">
         <v>71</v>
       </c>
@@ -6856,8 +6937,11 @@
       <c r="G27" s="24">
         <v>8.81</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="24">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="24" t="s">
         <v>71</v>
       </c>
@@ -6877,10 +6961,13 @@
         <v>0.71</v>
       </c>
       <c r="G28" s="24">
-        <v>8.2200000000000006</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="H28" s="24">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="24" t="s">
         <v>71</v>
       </c>
@@ -6900,10 +6987,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G29" s="24">
-        <v>10.53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>10.18</v>
+      </c>
+      <c r="H29" s="24">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="24" t="s">
         <v>71</v>
       </c>
@@ -6925,8 +7015,11 @@
       <c r="G30" s="24">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="24">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="24" t="s">
         <v>71</v>
       </c>
@@ -6948,8 +7041,11 @@
       <c r="G31" s="24">
         <v>11.51</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" s="24">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="24" t="s">
         <v>71</v>
       </c>
@@ -6969,10 +7065,13 @@
         <v>0.93</v>
       </c>
       <c r="G32" s="24">
-        <v>9.52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>9.82</v>
+      </c>
+      <c r="H32" s="24">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="24" t="s">
         <v>71</v>
       </c>
@@ -6992,10 +7091,13 @@
         <v>0.96</v>
       </c>
       <c r="G33" s="24">
-        <v>9.6999999999999993</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>9.35</v>
+      </c>
+      <c r="H33" s="24">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="24" t="s">
         <v>71</v>
       </c>
@@ -7015,10 +7117,13 @@
         <v>1</v>
       </c>
       <c r="G34" s="24">
-        <v>9.94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>10.24</v>
+      </c>
+      <c r="H34" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="24" t="s">
         <v>71</v>
       </c>
@@ -7038,10 +7143,13 @@
         <v>1.05</v>
       </c>
       <c r="G35" s="24">
-        <v>10.24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="H35" s="24">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="24" t="s">
         <v>71</v>
       </c>
@@ -7061,10 +7169,13 @@
         <v>1.06</v>
       </c>
       <c r="G36" s="24">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>8.16</v>
+      </c>
+      <c r="H36" s="24">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="24" t="s">
         <v>71</v>
       </c>
@@ -7084,10 +7195,13 @@
         <v>1</v>
       </c>
       <c r="G37" s="24">
-        <v>9.94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>10.24</v>
+      </c>
+      <c r="H37" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="24" t="s">
         <v>89</v>
       </c>
@@ -7107,10 +7221,13 @@
         <v>0.89</v>
       </c>
       <c r="G38" s="24">
-        <v>9.2899999999999991</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>9.35</v>
+      </c>
+      <c r="H38" s="24">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="24" t="s">
         <v>89</v>
       </c>
@@ -7130,10 +7247,13 @@
         <v>0.81</v>
       </c>
       <c r="G39" s="24">
-        <v>8.81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>9.94</v>
+      </c>
+      <c r="H39" s="24">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="24" t="s">
         <v>89</v>
       </c>
@@ -7153,10 +7273,13 @@
         <v>0.76</v>
       </c>
       <c r="G40" s="24">
-        <v>8.51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>8.4</v>
+      </c>
+      <c r="H40" s="24">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="24" t="s">
         <v>89</v>
       </c>
@@ -7176,10 +7299,13 @@
         <v>0.99</v>
       </c>
       <c r="G41" s="24">
-        <v>9.8800000000000008</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>10.24</v>
+      </c>
+      <c r="H41" s="24">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="24" t="s">
         <v>89</v>
       </c>
@@ -7199,10 +7325,13 @@
         <v>0.73</v>
       </c>
       <c r="G42" s="24">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>11.13</v>
+      </c>
+      <c r="H42" s="24">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="24" t="s">
         <v>89</v>
       </c>
@@ -7222,10 +7351,13 @@
         <v>0.77</v>
       </c>
       <c r="G43" s="24">
-        <v>8.57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H43" s="24">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="24" t="s">
         <v>89</v>
       </c>
@@ -7245,10 +7377,13 @@
         <v>0.95</v>
       </c>
       <c r="G44" s="24">
-        <v>9.64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="H44" s="24">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="24" t="s">
         <v>89</v>
       </c>
@@ -7268,10 +7403,13 @@
         <v>1.02</v>
       </c>
       <c r="G45" s="24">
-        <v>10.06</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>9.52</v>
+      </c>
+      <c r="H45" s="24">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="24" t="s">
         <v>89</v>
       </c>
@@ -7291,10 +7429,13 @@
         <v>0.82</v>
       </c>
       <c r="G46" s="24">
-        <v>8.8699999999999992</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="H46" s="24">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="24" t="s">
         <v>89</v>
       </c>
@@ -7314,10 +7455,13 @@
         <v>0.85</v>
       </c>
       <c r="G47" s="24">
-        <v>9.0500000000000007</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>10.18</v>
+      </c>
+      <c r="H47" s="24">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="24" t="s">
         <v>89</v>
       </c>
@@ -7337,10 +7481,13 @@
         <v>0.91</v>
       </c>
       <c r="G48" s="24">
-        <v>9.41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>10.06</v>
+      </c>
+      <c r="H48" s="24">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="24" t="s">
         <v>89</v>
       </c>
@@ -7360,10 +7507,13 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="G49" s="24">
-        <v>10.71</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="H49" s="24">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="24" t="s">
         <v>89</v>
       </c>
@@ -7383,10 +7533,13 @@
         <v>0.75</v>
       </c>
       <c r="G50" s="24">
-        <v>8.4600000000000009</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>8.99</v>
+      </c>
+      <c r="H50" s="24">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="24" t="s">
         <v>89</v>
       </c>
@@ -7406,10 +7559,13 @@
         <v>0.94</v>
       </c>
       <c r="G51" s="24">
-        <v>9.58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>10.06</v>
+      </c>
+      <c r="H51" s="24">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="24" t="s">
         <v>89</v>
       </c>
@@ -7431,8 +7587,11 @@
       <c r="G52" s="24">
         <v>10.06</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="H52" s="24">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="24" t="s">
         <v>89</v>
       </c>
@@ -7454,8 +7613,11 @@
       <c r="G53" s="24">
         <v>10.18</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="H53" s="24">
+        <v>-0.45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="24" t="s">
         <v>89</v>
       </c>
@@ -7475,10 +7637,13 @@
         <v>0.85</v>
       </c>
       <c r="G54" s="24">
-        <v>9.0500000000000007</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+        <v>7.21</v>
+      </c>
+      <c r="H54" s="24">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="24" t="s">
         <v>89</v>
       </c>
@@ -7498,10 +7663,13 @@
         <v>0.89</v>
       </c>
       <c r="G55" s="24">
-        <v>9.2899999999999991</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>9.94</v>
+      </c>
+      <c r="H55" s="24">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="24" t="s">
         <v>89</v>
       </c>
@@ -7521,10 +7689,13 @@
         <v>0.96</v>
       </c>
       <c r="G56" s="24">
-        <v>9.6999999999999993</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="H56" s="24">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="24" t="s">
         <v>89</v>
       </c>
@@ -7544,10 +7715,13 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="G57" s="24">
-        <v>4.0199999999999996</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+        <v>10.95</v>
+      </c>
+      <c r="H57" s="24">
+        <v>-0.77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="24" t="s">
         <v>89</v>
       </c>
@@ -7569,8 +7743,11 @@
       <c r="G58" s="24">
         <v>8.34</v>
       </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58" s="24">
+        <v>-0.82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="24" t="s">
         <v>89</v>
       </c>
@@ -7592,239 +7769,13 @@
       <c r="G59" s="24">
         <v>10.59</v>
       </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B60" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E60" s="24">
-        <v>50</v>
-      </c>
-      <c r="F60" s="7">
-        <v>0.36</v>
-      </c>
-      <c r="G60" s="24">
-        <v>6.14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B61" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D61" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" s="24">
-        <v>50</v>
-      </c>
-      <c r="F61" s="7">
-        <v>0.06</v>
-      </c>
-      <c r="G61" s="24">
-        <v>4.3600000000000003</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B62" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D62" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E62" s="24">
-        <v>50</v>
-      </c>
-      <c r="F62" s="7">
-        <v>0.47</v>
-      </c>
-      <c r="G62" s="24">
-        <v>6.79</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B63" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D63" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E63" s="24">
-        <v>50</v>
-      </c>
-      <c r="F63" s="7">
-        <v>0.39</v>
-      </c>
-      <c r="G63" s="24">
-        <v>6.32</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B64" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D64" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E64" s="24">
-        <v>50</v>
-      </c>
-      <c r="F64" s="7">
-        <v>0.48</v>
-      </c>
-      <c r="G64" s="24">
-        <v>6.85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B65" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D65" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E65" s="24">
-        <v>50</v>
-      </c>
-      <c r="F65" s="7">
-        <v>0.36</v>
-      </c>
-      <c r="G65" s="24">
-        <v>6.14</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B66" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D66" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E66" s="24">
-        <v>50</v>
-      </c>
-      <c r="F66" s="7">
-        <v>0.11</v>
-      </c>
-      <c r="G66" s="24">
-        <v>4.6500000000000004</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B67" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E67" s="24">
-        <v>50</v>
-      </c>
-      <c r="F67" s="7">
-        <v>0.15</v>
-      </c>
-      <c r="G67" s="24">
-        <v>4.8899999999999997</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B68" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D68" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E68" s="24">
-        <v>70</v>
-      </c>
-      <c r="F68" s="7">
-        <v>0.11</v>
-      </c>
-      <c r="G68" s="24">
-        <v>4.6500000000000004</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B69" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D69" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E69" s="24">
-        <v>70</v>
-      </c>
-      <c r="F69" s="7">
-        <v>0.11</v>
-      </c>
-      <c r="G69" s="24">
-        <v>4.6500000000000004</v>
+      <c r="H59" s="24">
+        <v>-0.6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>